<commit_message>
Finish report and add comments to code
</commit_message>
<xml_diff>
--- a/amortization_table.xlsx
+++ b/amortization_table.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kary\Documents\semestre_8\lenguajes_programacion\programming_lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32D3C6-7A2A-4E3D-A270-7D28E7796FDC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5168B498-F7FB-4FEA-A8FF-D7DCA461AAF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DA39A20F-7967-494C-90D3-3EE9E99A69F6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jack's bf" sheetId="1" r:id="rId1"/>
+    <sheet name="Example" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -174,9 +174,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -187,6 +184,9 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -507,7 +507,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,14 +521,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -540,7 +540,7 @@
       <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <f>B12</f>
         <v>95044.203263909265</v>
       </c>
@@ -555,7 +555,7 @@
       <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f>C24</f>
         <v>140530.43916691092</v>
       </c>
@@ -570,7 +570,7 @@
       <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <f>B24</f>
         <v>1140530.4391669114</v>
       </c>
@@ -613,7 +613,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="1"/>
       <c r="F11" s="3">
         <f>B3</f>
@@ -625,27 +625,27 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <f t="shared" ref="B12:B23" si="0">PMT($B$6,$B$4,-$B$3)</f>
         <v>95044.203263909265</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <f t="shared" ref="C12:C23" si="1">F11*$B$6</f>
         <v>20833.333333333332</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f>C12</f>
         <v>20833.333333333332</v>
       </c>
-      <c r="E12" s="13">
-        <f t="shared" ref="E12:E24" si="2">B12-C12</f>
+      <c r="E12" s="12">
+        <f t="shared" ref="E12:E23" si="2">B12-C12</f>
         <v>74210.869930575936</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <f>F11-E12</f>
         <v>925789.13006942405</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <f>G11+E12</f>
         <v>74210.869930575936</v>
       </c>
@@ -654,27 +654,27 @@
       <c r="A13" s="1">
         <v>2</v>
       </c>
-      <c r="B13" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C13" s="14">
+      <c r="B13" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C13" s="13">
         <f t="shared" si="1"/>
         <v>19287.273543112999</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <f>C13+D12</f>
         <v>40120.606876446327</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <f t="shared" si="2"/>
         <v>75756.929720796266</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <f t="shared" ref="F13:F23" si="3">F12-E13</f>
         <v>850032.20034862775</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <f t="shared" ref="G13:G23" si="4">G12+E13</f>
         <v>149967.79965137219</v>
       </c>
@@ -683,27 +683,27 @@
       <c r="A14" s="1">
         <v>3</v>
       </c>
-      <c r="B14" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C14" s="14">
+      <c r="B14" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C14" s="13">
         <f t="shared" si="1"/>
         <v>17709.004173929745</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <f t="shared" ref="D14:D23" si="5">C14+D13</f>
         <v>57829.611050376072</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <f t="shared" si="2"/>
         <v>77335.19908997952</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <f t="shared" si="3"/>
         <v>772697.00125864823</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <f t="shared" si="4"/>
         <v>227302.99874135171</v>
       </c>
@@ -712,27 +712,27 @@
       <c r="A15" s="1">
         <v>4</v>
       </c>
-      <c r="B15" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C15" s="14">
+      <c r="B15" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C15" s="13">
         <f t="shared" si="1"/>
         <v>16097.854192888504</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <f t="shared" si="5"/>
         <v>73927.465243264582</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <f t="shared" si="2"/>
         <v>78946.349071020755</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
         <f t="shared" si="3"/>
         <v>693750.65218762751</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <f t="shared" si="4"/>
         <v>306249.34781237249</v>
       </c>
@@ -741,27 +741,27 @@
       <c r="A16" s="1">
         <v>5</v>
       </c>
-      <c r="B16" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C16" s="14">
+      <c r="B16" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C16" s="13">
         <f t="shared" si="1"/>
         <v>14453.13858724224</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <f t="shared" si="5"/>
         <v>88380.603830506821</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <f t="shared" si="2"/>
         <v>80591.064676667025</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <f t="shared" si="3"/>
         <v>613159.58751096053</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="12">
         <f t="shared" si="4"/>
         <v>386840.41248903953</v>
       </c>
@@ -770,27 +770,27 @@
       <c r="A17" s="1">
         <v>6</v>
       </c>
-      <c r="B17" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C17" s="14">
+      <c r="B17" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C17" s="13">
         <f t="shared" si="1"/>
         <v>12774.15807314501</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <f t="shared" si="5"/>
         <v>101154.76190365183</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <f t="shared" si="2"/>
         <v>82270.045190764256</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <f t="shared" si="3"/>
         <v>530889.54232019628</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="12">
         <f t="shared" si="4"/>
         <v>469110.45767980377</v>
       </c>
@@ -799,27 +799,27 @@
       <c r="A18" s="1">
         <v>7</v>
       </c>
-      <c r="B18" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C18" s="14">
+      <c r="B18" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C18" s="13">
         <f t="shared" si="1"/>
         <v>11060.198798337422</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <f t="shared" si="5"/>
         <v>112214.96070198926</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <f t="shared" si="2"/>
         <v>83984.004465571837</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <f t="shared" si="3"/>
         <v>446905.53785462445</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <f t="shared" si="4"/>
         <v>553094.46214537555</v>
       </c>
@@ -828,27 +828,27 @@
       <c r="A19" s="1">
         <v>8</v>
       </c>
-      <c r="B19" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C19" s="14">
+      <c r="B19" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C19" s="13">
         <f t="shared" si="1"/>
         <v>9310.5320386380081</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <f t="shared" si="5"/>
         <v>121525.49274062726</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <f t="shared" si="2"/>
         <v>85733.67122527126</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <f t="shared" si="3"/>
         <v>361171.8666293532</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <f t="shared" si="4"/>
         <v>638828.13337064686</v>
       </c>
@@ -857,27 +857,27 @@
       <c r="A20" s="1">
         <v>9</v>
       </c>
-      <c r="B20" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C20" s="14">
+      <c r="B20" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C20" s="13">
         <f t="shared" si="1"/>
         <v>7524.413888111525</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="10">
         <f t="shared" si="5"/>
         <v>129049.90662873878</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <f t="shared" si="2"/>
         <v>87519.789375797744</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f t="shared" si="3"/>
         <v>273652.07725355547</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <f t="shared" si="4"/>
         <v>726347.92274644459</v>
       </c>
@@ -886,27 +886,27 @@
       <c r="A21" s="1">
         <v>10</v>
       </c>
-      <c r="B21" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C21" s="14">
+      <c r="B21" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C21" s="13">
         <f t="shared" si="1"/>
         <v>5701.0849427824051</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="10">
         <f t="shared" si="5"/>
         <v>134750.99157152118</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <f t="shared" si="2"/>
         <v>89343.118321126865</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <f t="shared" si="3"/>
         <v>184308.95893242862</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <f t="shared" si="4"/>
         <v>815691.0410675715</v>
       </c>
@@ -915,27 +915,27 @@
       <c r="A22" s="1">
         <v>11</v>
       </c>
-      <c r="B22" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C22" s="14">
+      <c r="B22" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C22" s="13">
         <f t="shared" si="1"/>
         <v>3839.7699777589296</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="10">
         <f t="shared" si="5"/>
         <v>138590.76154928011</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <f t="shared" si="2"/>
         <v>91204.433286150335</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <f t="shared" si="3"/>
         <v>93104.525646278285</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="12">
         <f t="shared" si="4"/>
         <v>906895.47435372183</v>
       </c>
@@ -944,27 +944,27 @@
       <c r="A23" s="1">
         <v>12</v>
       </c>
-      <c r="B23" s="13">
-        <f t="shared" si="0"/>
-        <v>95044.203263909265</v>
-      </c>
-      <c r="C23" s="14">
+      <c r="B23" s="12">
+        <f t="shared" si="0"/>
+        <v>95044.203263909265</v>
+      </c>
+      <c r="C23" s="13">
         <f t="shared" si="1"/>
         <v>1939.6776176307976</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <f t="shared" si="5"/>
         <v>140530.43916691092</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <f t="shared" si="2"/>
         <v>93104.52564627846</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <f t="shared" si="3"/>
         <v>-1.7462298274040222E-10</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <f t="shared" si="4"/>
         <v>1000000.0000000002</v>
       </c>
@@ -974,11 +974,11 @@
         <f>SUM(B12:B23)</f>
         <v>1140530.4391669114</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <f>SUM(C12:C23)</f>
         <v>140530.43916691092</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>